<commit_message>
Re-writting test in pytest
</commit_message>
<xml_diff>
--- a/app/test/test_data/raw_test_data.xlsx
+++ b/app/test/test_data/raw_test_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -840,27 +840,27 @@
   </sheetPr>
   <dimension ref="A1:Q65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O7" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B:B"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="22:22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="17.0890688259109"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.2591093117409"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="23.8866396761134"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="12.6761133603239"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="14.6761133603239"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="23.4574898785425"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="23.0323886639676"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="30.1012145748988"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="38.5627530364372"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="32.9919028340081"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="34.3846153846154"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="42.4210526315789"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="27.4210526315789"/>
-    <col collapsed="false" hidden="false" max="16" min="15" style="1" width="26.1376518218623"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="15.3198380566802"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="17.4615384615385"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.3886639676113"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="24.5303643724696"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="12.9595141700405"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="14.9959514170041"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="23.8866396761134"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="23.3522267206478"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="30.7449392712551"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="39.5263157894737"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="33.8502024291498"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="35.0283400809717"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="43.5991902834008"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="28.0647773279352"/>
+    <col collapsed="false" hidden="false" max="16" min="15" style="1" width="26.7813765182186"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="15.6396761133603"/>
     <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="10.6032388663968"/>
   </cols>
   <sheetData>
@@ -917,7 +917,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>17</v>
       </c>
@@ -1817,7 +1817,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
         <v>203</v>
       </c>
@@ -1917,6 +1917,9 @@
         <v>73</v>
       </c>
     </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1044549" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1044550" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1044551" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1044552" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -5963,7 +5966,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B:B A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="22:22 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5989,7 +5992,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B:B A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="22:22 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>